<commit_message>
Remove dangling .lock file
and changed the case on a version "v".
</commit_message>
<xml_diff>
--- a/POSCON.ECO.xlsx
+++ b/POSCON.ECO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -70,7 +70,7 @@
     <t>Consistent naming</t>
   </si>
   <si>
-    <t>POSCON.V1.2</t>
+    <t>POSCON.v1.2</t>
   </si>
   <si>
     <t>Changes to POSCON.FACE &amp; POSCON.BACK, added new part POSCON.CORE. New mounting schema. (Snaps)</t>
@@ -113,13 +113,13 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -175,12 +175,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -188,19 +192,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -224,7 +220,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -290,7 +286,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
+      <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -305,7 +301,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
+      <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
@@ -323,13 +319,13 @@
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E6" s="4" t="n">
@@ -337,32 +333,32 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -393,74 +389,74 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -491,74 +487,74 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Removed Ver 1.2 Rev C fileset, Added Ver 1.3 Rev D fileset
</commit_message>
<xml_diff>
--- a/POSCON.ECO.xlsx
+++ b/POSCON.ECO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>Release ID</t>
   </si>
@@ -80,17 +80,27 @@
   </si>
   <si>
     <t>New parts, redesign POSCON.BACK &amp; POSCON.FACE, delete superseded parts</t>
+  </si>
+  <si>
+    <t>POSCON.v1.3</t>
+  </si>
+  <si>
+    <t>Added 0.031” radius to notches on back of POSCON.FACE</t>
+  </si>
+  <si>
+    <t>First articles came back from vendor with radiused notches, drawing change made to reduce future potential for confusion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
+    <numFmt numFmtId="166" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
@@ -113,8 +123,14 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
-      <sz val="11"/>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -175,29 +191,45 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -220,145 +252,155 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.5"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="40.8777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.2518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="36.2777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.0037037037037"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="6.62592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="6.62592592592593"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="44.3666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.0481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="49.7333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.62962962962963"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.07407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="2" width="7.07407407407407"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="n">
+      <c r="E2" s="5" t="n">
         <v>41925</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4" t="n">
+      <c r="E3" s="5" t="n">
         <v>41927</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="4" t="n">
+      <c r="E4" s="5" t="n">
         <v>41927</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="4" t="n">
+      <c r="E5" s="5" t="n">
         <v>41927</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="31" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4" t="n">
+      <c r="E6" s="5" t="n">
         <v>42132</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>42256</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -384,79 +426,79 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="256" min="1" style="1" width="6.62592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="6.62592592592593"/>
+    <col collapsed="false" hidden="false" max="256" min="1" style="8" width="7.07407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.07407407407407"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -482,79 +524,79 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="256" min="1" style="1" width="6.62592592592593"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="6.62592592592593"/>
+    <col collapsed="false" hidden="false" max="256" min="1" style="8" width="7.07407407407407"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.07407407407407"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Copied commit messages to ECO
</commit_message>
<xml_diff>
--- a/POSCON.ECO.xlsx
+++ b/POSCON.ECO.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Release ID</t>
   </si>
@@ -89,6 +89,12 @@
   </si>
   <si>
     <t>First articles came back from vendor with radiused notches, drawing change made to reduce future potential for confusion</t>
+  </si>
+  <si>
+    <t>Corrected date on drawing to 09/09/2015</t>
+  </si>
+  <si>
+    <t>Good data hygiene</t>
   </si>
 </sst>
 </file>
@@ -123,13 +129,13 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -191,41 +197,37 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -251,19 +253,19 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2703703703704"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="44.3666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.0481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="49.7333333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.62962962962963"/>
-    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.07407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="2" width="7.07407407407407"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.0481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="48.0740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.9962962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="53.9407407407408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.32222222222222"/>
+    <col collapsed="false" hidden="false" max="256" min="6" style="1" width="7.5962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="2" width="7.5962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -383,10 +385,18 @@
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>42257</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
@@ -426,79 +436,79 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="256" min="1" style="8" width="7.07407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.07407407407407"/>
+    <col collapsed="false" hidden="false" max="256" min="1" style="1" width="7.5962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.5962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -524,79 +534,79 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="256" min="1" style="8" width="7.07407407407407"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.07407407407407"/>
+    <col collapsed="false" hidden="false" max="256" min="1" style="1" width="7.5962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="7.5962962962963"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9"/>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>